<commit_message>
Excel Dary basic status
</commit_message>
<xml_diff>
--- a/Dairy.xlsx
+++ b/Dairy.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\bitcelolDiaryTHing\BitCell_Dairy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6884B6C-BC73-4480-A2E7-E8E8D3BD13B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Time and Date</t>
+  </si>
+  <si>
+    <t>What I've done</t>
+  </si>
+  <si>
+    <t>How long</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +48,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,14 +125,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +487,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>